<commit_message>
[FEATURE] add visual filter by status
</commit_message>
<xml_diff>
--- a/webapp/localService/metadata.xlsx
+++ b/webapp/localService/metadata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="930" yWindow="0" windowWidth="27870" windowHeight="12915" activeTab="2"/>
+    <workbookView xWindow="930" yWindow="0" windowWidth="27870" windowHeight="12915" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ActDataSet" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="121">
   <si>
     <t>ID</t>
   </si>
@@ -328,6 +328,9 @@
   </si>
   <si>
     <t>StatusText</t>
+  </si>
+  <si>
+    <t>PartnersInStatus</t>
   </si>
   <si>
     <t>Project</t>
@@ -453,14 +456,16 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="StatusSet" displayName="StatusSet" ref="A1:B4">
-  <autoFilter ref="A1:B4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="StatusSet" displayName="StatusSet" ref="A1:C4">
+  <autoFilter ref="A1:C4">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
   </autoFilter>
-  <tableColumns count="2">
+  <tableColumns count="3">
     <tableColumn id="1" name="StatusID" totalsRowLabel="Total"/>
     <tableColumn id="2" name="StatusText"/>
+    <tableColumn id="3" name="PartnersInStatus"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -1785,45 +1790,59 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="20" customWidth="1"/>
+    <col min="1" max="3" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>102</v>
       </c>
       <c r="B1" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+      <c r="C2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+      <c r="C3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>106</v>
+        <v>107</v>
+      </c>
+      <c r="C4">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -1839,9 +1858,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="A3:C11"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1850,13 +1867,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -1864,7 +1881,7 @@
         <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C2">
         <v>3</v>
@@ -1875,7 +1892,7 @@
         <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C3">
         <v>4</v>
@@ -1886,7 +1903,7 @@
         <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C4">
         <v>7</v>
@@ -1897,7 +1914,7 @@
         <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C5">
         <v>9</v>
@@ -1908,7 +1925,7 @@
         <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C6">
         <v>8</v>
@@ -1919,7 +1936,7 @@
         <v>21</v>
       </c>
       <c r="B7" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C7">
         <v>3</v>
@@ -1930,7 +1947,7 @@
         <v>24</v>
       </c>
       <c r="B8" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C8">
         <v>4</v>
@@ -1941,7 +1958,7 @@
         <v>27</v>
       </c>
       <c r="B9" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C9">
         <v>5</v>
@@ -1952,7 +1969,7 @@
         <v>30</v>
       </c>
       <c r="B10" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C10">
         <v>6</v>
@@ -1963,7 +1980,7 @@
         <v>33</v>
       </c>
       <c r="B11" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C11">
         <v>4</v>

</xml_diff>

<commit_message>
[FEATURE] add visual filter for start date
</commit_message>
<xml_diff>
--- a/webapp/localService/metadata.xlsx
+++ b/webapp/localService/metadata.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="930" yWindow="0" windowWidth="27870" windowHeight="12915" activeTab="1"/>
+    <workbookView xWindow="2790" yWindow="0" windowWidth="27870" windowHeight="12915" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="ActDataSet" sheetId="1" r:id="rId1"/>
     <sheet name="StatusSet" sheetId="2" r:id="rId2"/>
     <sheet name="PartnerSet" sheetId="3" r:id="rId3"/>
+    <sheet name="DateFilterSet" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="174">
   <si>
     <t>ID</t>
   </si>
@@ -36,6 +37,9 @@
     <t>Sum</t>
   </si>
   <si>
+    <t>StartDate</t>
+  </si>
+  <si>
     <t>1</t>
   </si>
   <si>
@@ -379,6 +383,162 @@
   </si>
   <si>
     <t>Amazon</t>
+  </si>
+  <si>
+    <t>ProcessedAct</t>
+  </si>
+  <si>
+    <t>20210510</t>
+  </si>
+  <si>
+    <t>20210501</t>
+  </si>
+  <si>
+    <t>20200101</t>
+  </si>
+  <si>
+    <t>20200110</t>
+  </si>
+  <si>
+    <t>20200120</t>
+  </si>
+  <si>
+    <t>20200201</t>
+  </si>
+  <si>
+    <t>20200210</t>
+  </si>
+  <si>
+    <t>20200220</t>
+  </si>
+  <si>
+    <t>20200301</t>
+  </si>
+  <si>
+    <t>20200310</t>
+  </si>
+  <si>
+    <t>20200320</t>
+  </si>
+  <si>
+    <t>20200401</t>
+  </si>
+  <si>
+    <t>20200410</t>
+  </si>
+  <si>
+    <t>20200420</t>
+  </si>
+  <si>
+    <t>20200501</t>
+  </si>
+  <si>
+    <t>20200510</t>
+  </si>
+  <si>
+    <t>20200520</t>
+  </si>
+  <si>
+    <t>20200601</t>
+  </si>
+  <si>
+    <t>20200610</t>
+  </si>
+  <si>
+    <t>20200620</t>
+  </si>
+  <si>
+    <t>20200701</t>
+  </si>
+  <si>
+    <t>20200710</t>
+  </si>
+  <si>
+    <t>20200720</t>
+  </si>
+  <si>
+    <t>20200801</t>
+  </si>
+  <si>
+    <t>20200810</t>
+  </si>
+  <si>
+    <t>20200820</t>
+  </si>
+  <si>
+    <t>20200901</t>
+  </si>
+  <si>
+    <t>20200910</t>
+  </si>
+  <si>
+    <t>20200920</t>
+  </si>
+  <si>
+    <t>20201001</t>
+  </si>
+  <si>
+    <t>20201010</t>
+  </si>
+  <si>
+    <t>20201020</t>
+  </si>
+  <si>
+    <t>20201101</t>
+  </si>
+  <si>
+    <t>20201110</t>
+  </si>
+  <si>
+    <t>20201120</t>
+  </si>
+  <si>
+    <t>20201201</t>
+  </si>
+  <si>
+    <t>20201210</t>
+  </si>
+  <si>
+    <t>20201220</t>
+  </si>
+  <si>
+    <t>20210101</t>
+  </si>
+  <si>
+    <t>20210110</t>
+  </si>
+  <si>
+    <t>20210120</t>
+  </si>
+  <si>
+    <t>20210201</t>
+  </si>
+  <si>
+    <t>20210210</t>
+  </si>
+  <si>
+    <t>20210220</t>
+  </si>
+  <si>
+    <t>20210301</t>
+  </si>
+  <si>
+    <t>20210310</t>
+  </si>
+  <si>
+    <t>20210320</t>
+  </si>
+  <si>
+    <t>20210401</t>
+  </si>
+  <si>
+    <t>20210410</t>
+  </si>
+  <si>
+    <t>20210420</t>
+  </si>
+  <si>
+    <t>2</t>
   </si>
 </sst>
 </file>
@@ -414,13 +574,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -434,22 +602,24 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="ActDataSet" displayName="ActDataSet" ref="A1:F51">
-  <autoFilter ref="A1:F51">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="ActDataSet" displayName="ActDataSet" ref="A1:G51">
+  <autoFilter ref="A1:G51">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
     <filterColumn colId="3" hiddenButton="1"/>
     <filterColumn colId="4" hiddenButton="1"/>
     <filterColumn colId="5" hiddenButton="1"/>
+    <filterColumn colId="6" hiddenButton="1"/>
   </autoFilter>
-  <tableColumns count="6">
+  <tableColumns count="7">
     <tableColumn id="1" name="ID" totalsRowLabel="Total"/>
     <tableColumn id="2" name="Partner"/>
     <tableColumn id="3" name="Status"/>
     <tableColumn id="4" name="Title"/>
     <tableColumn id="5" name="Count"/>
     <tableColumn id="6" name="Sum"/>
+    <tableColumn id="7" name="StartDate" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -482,6 +652,20 @@
     <tableColumn id="1" name="PartnerID" totalsRowLabel="Total"/>
     <tableColumn id="2" name="PartnerText"/>
     <tableColumn id="3" name="Rating"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="DateFilterSet" displayName="DateFilterSet" ref="A1:B51">
+  <autoFilter ref="A1:B51">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="2">
+    <tableColumn id="1" name="StartDate" totalsRowLabel="Total" dataDxfId="0"/>
+    <tableColumn id="2" name="ProcessedAct"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -750,16 +934,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F51"/>
+  <dimension ref="A1:G51"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="6" width="20" customWidth="1"/>
+    <col min="1" max="7" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -778,19 +964,22 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E2">
         <v>16</v>
@@ -798,19 +987,22 @@
       <c r="F2">
         <v>2188</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
+      <c r="G2" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>173</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E3">
         <v>35</v>
@@ -818,19 +1010,22 @@
       <c r="F3">
         <v>4466</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E4">
         <v>6</v>
@@ -838,19 +1033,22 @@
       <c r="F4">
         <v>1549</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E5">
         <v>42</v>
@@ -858,19 +1056,22 @@
       <c r="F5">
         <v>2802</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E6">
         <v>89</v>
@@ -878,19 +1079,22 @@
       <c r="F6">
         <v>1331</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G6" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D7" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E7">
         <v>18</v>
@@ -898,19 +1102,22 @@
       <c r="F7">
         <v>380</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G7" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C8" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E8">
         <v>70</v>
@@ -918,19 +1125,22 @@
       <c r="F8">
         <v>2248</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G8" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B9" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C9" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E9">
         <v>84</v>
@@ -938,19 +1148,22 @@
       <c r="F9">
         <v>834</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G9" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B10" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C10" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D10" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E10">
         <v>11</v>
@@ -958,19 +1171,22 @@
       <c r="F10">
         <v>2373</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G10" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B11" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C11" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D11" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E11">
         <v>50</v>
@@ -978,19 +1194,22 @@
       <c r="F11">
         <v>2661</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G11" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B12" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C12" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D12" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E12">
         <v>62</v>
@@ -998,19 +1217,22 @@
       <c r="F12">
         <v>876</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G12" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B13" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C13" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D13" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E13">
         <v>74</v>
@@ -1018,19 +1240,22 @@
       <c r="F13">
         <v>3467</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G13" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B14" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D14" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E14">
         <v>64</v>
@@ -1038,19 +1263,22 @@
       <c r="F14">
         <v>4970</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G14" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B15" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C15" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D15" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E15">
         <v>28</v>
@@ -1058,19 +1286,22 @@
       <c r="F15">
         <v>3558</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G15" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B16" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C16" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D16" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E16">
         <v>49</v>
@@ -1078,19 +1309,22 @@
       <c r="F16">
         <v>3543</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G16" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B17" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C17" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D17" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E17">
         <v>74</v>
@@ -1098,19 +1332,22 @@
       <c r="F17">
         <v>853</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G17" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B18" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C18" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D18" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E18">
         <v>46</v>
@@ -1118,19 +1355,22 @@
       <c r="F18">
         <v>2392</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G18" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B19" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C19" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D19" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E19">
         <v>42</v>
@@ -1138,19 +1378,22 @@
       <c r="F19">
         <v>2571</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G19" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B20" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C20" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D20" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E20">
         <v>93</v>
@@ -1158,19 +1401,22 @@
       <c r="F20">
         <v>491</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G20" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B21" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C21" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D21" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E21">
         <v>86</v>
@@ -1178,19 +1424,22 @@
       <c r="F21">
         <v>3847</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G21" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B22" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C22" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D22" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E22">
         <v>53</v>
@@ -1198,19 +1447,22 @@
       <c r="F22">
         <v>1357</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G22" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B23" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C23" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D23" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E23">
         <v>20</v>
@@ -1218,19 +1470,22 @@
       <c r="F23">
         <v>2893</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G23" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B24" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C24" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D24" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E24">
         <v>61</v>
@@ -1238,19 +1493,22 @@
       <c r="F24">
         <v>2485</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G24" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B25" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C25" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D25" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E25">
         <v>32</v>
@@ -1258,19 +1516,22 @@
       <c r="F25">
         <v>4859</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G25" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B26" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C26" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D26" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E26">
         <v>65</v>
@@ -1278,19 +1539,22 @@
       <c r="F26">
         <v>2552</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G26" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B27" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C27" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D27" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E27">
         <v>88</v>
@@ -1298,19 +1562,22 @@
       <c r="F27">
         <v>4108</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G27" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B28" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C28" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D28" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E28">
         <v>96</v>
@@ -1318,19 +1585,22 @@
       <c r="F28">
         <v>2262</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G28" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B29" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C29" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D29" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E29">
         <v>52</v>
@@ -1338,19 +1608,22 @@
       <c r="F29">
         <v>3784</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G29" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B30" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C30" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D30" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E30">
         <v>13</v>
@@ -1358,19 +1631,22 @@
       <c r="F30">
         <v>4178</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G30" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B31" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C31" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D31" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E31">
         <v>17</v>
@@ -1378,19 +1654,22 @@
       <c r="F31">
         <v>417</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G31" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B32" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C32" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D32" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E32">
         <v>84</v>
@@ -1398,19 +1677,22 @@
       <c r="F32">
         <v>4310</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G32" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B33" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C33" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D33" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E33">
         <v>20</v>
@@ -1418,19 +1700,22 @@
       <c r="F33">
         <v>3684</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G33" s="1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B34" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C34" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D34" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E34">
         <v>8</v>
@@ -1438,19 +1723,22 @@
       <c r="F34">
         <v>1466</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G34" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B35" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C35" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D35" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E35">
         <v>26</v>
@@ -1458,19 +1746,22 @@
       <c r="F35">
         <v>364</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G35" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B36" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C36" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D36" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="E36">
         <v>39</v>
@@ -1478,19 +1769,22 @@
       <c r="F36">
         <v>1495</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G36" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B37" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C37" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D37" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E37">
         <v>33</v>
@@ -1498,19 +1792,22 @@
       <c r="F37">
         <v>4230</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G37" s="1" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B38" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C38" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D38" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E38">
         <v>9</v>
@@ -1518,19 +1815,22 @@
       <c r="F38">
         <v>2089</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G38" s="1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B39" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C39" t="s">
+        <v>10</v>
+      </c>
+      <c r="D39" t="s">
         <v>9</v>
-      </c>
-      <c r="D39" t="s">
-        <v>8</v>
       </c>
       <c r="E39">
         <v>32</v>
@@ -1538,19 +1838,22 @@
       <c r="F39">
         <v>3627</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G39" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B40" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C40" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D40" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E40">
         <v>65</v>
@@ -1558,19 +1861,22 @@
       <c r="F40">
         <v>4890</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G40" s="1" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B41" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C41" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D41" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E41">
         <v>74</v>
@@ -1578,19 +1884,22 @@
       <c r="F41">
         <v>3503</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G41" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B42" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C42" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D42" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E42">
         <v>50</v>
@@ -1598,19 +1907,22 @@
       <c r="F42">
         <v>3154</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G42" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B43" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C43" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D43" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E43">
         <v>77</v>
@@ -1618,19 +1930,22 @@
       <c r="F43">
         <v>1992</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G43" s="1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B44" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C44" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D44" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E44">
         <v>37</v>
@@ -1638,19 +1953,22 @@
       <c r="F44">
         <v>4372</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G44" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B45" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C45" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D45" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E45">
         <v>89</v>
@@ -1658,19 +1976,22 @@
       <c r="F45">
         <v>4836</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G45" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B46" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C46" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D46" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E46">
         <v>66</v>
@@ -1678,19 +1999,22 @@
       <c r="F46">
         <v>2661</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G46" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B47" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C47" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D47" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E47">
         <v>82</v>
@@ -1698,19 +2022,22 @@
       <c r="F47">
         <v>4129</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G47" s="1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B48" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C48" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D48" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E48">
         <v>7</v>
@@ -1718,19 +2045,22 @@
       <c r="F48">
         <v>4666</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G48" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B49" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C49" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D49" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E49">
         <v>82</v>
@@ -1738,19 +2068,22 @@
       <c r="F49">
         <v>1635</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G49" s="1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B50" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C50" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D50" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E50">
         <v>89</v>
@@ -1758,25 +2091,31 @@
       <c r="F50">
         <v>2951</v>
       </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G50" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B51" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C51" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D51" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E51">
         <v>65</v>
       </c>
       <c r="F51">
         <v>4081</v>
+      </c>
+      <c r="G51" s="1" t="s">
+        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -1792,9 +2131,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1803,21 +2140,21 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C2">
         <v>12</v>
@@ -1825,10 +2162,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C3">
         <v>23</v>
@@ -1836,10 +2173,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C4">
         <v>15</v>
@@ -1867,21 +2204,21 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C2">
         <v>3</v>
@@ -1889,10 +2226,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C3">
         <v>4</v>
@@ -1900,10 +2237,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C4">
         <v>7</v>
@@ -1911,10 +2248,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C5">
         <v>9</v>
@@ -1922,10 +2259,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B6" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C6">
         <v>8</v>
@@ -1933,10 +2270,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B7" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C7">
         <v>3</v>
@@ -1944,10 +2281,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B8" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C8">
         <v>4</v>
@@ -1955,10 +2292,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B9" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C9">
         <v>5</v>
@@ -1966,10 +2303,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B10" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C10">
         <v>6</v>
@@ -1977,13 +2314,443 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B11" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C11">
         <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B51"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D47" sqref="D47"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="20" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B5">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B6">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B7">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B8">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B9">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B10">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B11">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B12">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B13">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B14">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B15">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B16">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B17">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B18">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B19">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B20">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B21">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B22">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B23">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="B24">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B26">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="B27">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="B28">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="B29">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B30">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B31">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B32">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="B33">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="B34">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B35">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="B36">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B37">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="B38">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B39">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B40">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="B41">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B42">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B43">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="B44">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B45">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="B46">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="B47">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="B48">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="B49">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B50">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B51">
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>